<commit_message>
edit 1 vai cai
</commit_message>
<xml_diff>
--- a/CinemaProject_New/ThongKe_DoanhThu.xlsx
+++ b/CinemaProject_New/ThongKe_DoanhThu.xlsx
@@ -12,9 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Thống kê từ ngày 2025-05-22 đến 2025-06-29</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Thống kê từ ngày 2025-05-23 đến 2026-06-01</t>
   </si>
   <si>
     <t>Tên phim</t>
@@ -29,28 +29,31 @@
     <t>Doanh thu (VNĐ)</t>
   </si>
   <si>
+    <t>Mario Bros</t>
+  </si>
+  <si>
     <t>Rocky</t>
   </si>
   <si>
+    <t>Ant-Man</t>
+  </si>
+  <si>
+    <t>Avengers</t>
+  </si>
+  <si>
+    <t>Immaculate</t>
+  </si>
+  <si>
     <t>Ròm</t>
   </si>
   <si>
-    <t>Ant-Man</t>
-  </si>
-  <si>
-    <t>Avenger</t>
-  </si>
-  <si>
-    <t>Immaculate</t>
-  </si>
-  <si>
-    <t>Mario Bros</t>
+    <t>The Lion King</t>
   </si>
   <si>
     <t>Tổng doanh thu:</t>
   </si>
   <si>
-    <t>980000</t>
+    <t>1030000</t>
   </si>
 </sst>
 </file>
@@ -95,7 +98,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -134,10 +137,10 @@
         <v>4.0</v>
       </c>
       <c r="C4" t="n" s="0">
-        <v>10.0</v>
+        <v>13.0</v>
       </c>
       <c r="D4" t="n" s="0">
-        <v>700000.0</v>
+        <v>750000.0</v>
       </c>
     </row>
     <row r="5">
@@ -145,7 +148,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="C5" t="n" s="0">
         <v>4.0</v>
@@ -159,7 +162,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="n" s="0">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="C6" t="n" s="0">
         <v>0.0</v>
@@ -173,7 +176,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="n" s="0">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C7" t="n" s="0">
         <v>0.0</v>
@@ -187,7 +190,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="n" s="0">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
       <c r="C8" t="n" s="0">
         <v>0.0</v>
@@ -201,7 +204,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="n" s="0">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c r="C9" t="n" s="0">
         <v>0.0</v>
@@ -210,12 +213,26 @@
         <v>0.0</v>
       </c>
     </row>
-    <row r="11">
-      <c r="C11" t="s" s="0">
+    <row r="10">
+      <c r="A10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D11" t="s" s="0">
+      <c r="B10" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" t="s" s="0">
         <v>12</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>